<commit_message>
Annex überarbeitet und Auswertung angefangen
</commit_message>
<xml_diff>
--- a/Findings.xlsx
+++ b/Findings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -151,12 +151,6 @@
     <t>sachlich</t>
   </si>
   <si>
-    <t>Tapferkeit</t>
-  </si>
-  <si>
-    <t>Selbständigkeit</t>
-  </si>
-  <si>
     <t>selbstlos</t>
   </si>
   <si>
@@ -167,6 +161,12 @@
   </si>
   <si>
     <t>empathisch</t>
+  </si>
+  <si>
+    <t>tapfer</t>
+  </si>
+  <si>
+    <t>selbständig</t>
   </si>
 </sst>
 </file>
@@ -1461,10 +1461,10 @@
                   <c:v>sachlich</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Tapferkeit</c:v>
+                  <c:v>tapfer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Selbständigkeit</c:v>
+                  <c:v>selbständig</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Ehe</c:v>
@@ -1616,10 +1616,10 @@
                   <c:v>sachlich</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Tapferkeit</c:v>
+                  <c:v>tapfer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Selbständigkeit</c:v>
+                  <c:v>selbständig</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Ehe</c:v>
@@ -3560,7 +3560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB62"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AP1" activePane="topRight" state="frozenSplit"/>
       <selection sqref="A1 C1:C1048576"/>
       <selection pane="topRight" activeCell="B42" sqref="B42:Z62"/>
@@ -7659,8 +7659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7723,7 +7723,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>19</v>
@@ -7734,7 +7734,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -7756,7 +7756,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -7811,7 +7811,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -7822,7 +7822,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -7855,7 +7855,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -7885,7 +7885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>